<commit_message>
busquedaSimple funcionando! no tocar
</commit_message>
<xml_diff>
--- a/docPDS/Estimacion_Proyecto.xlsx
+++ b/docPDS/Estimacion_Proyecto.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BorisMR\git\PDS-CRM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspace\PDS-CRM\docPDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>Número</t>
   </si>
@@ -307,16 +307,13 @@
     <t>Login Fallido</t>
   </si>
   <si>
-    <t>Buscador Simple</t>
-  </si>
-  <si>
-    <t>Buscador Avanzado</t>
-  </si>
-  <si>
-    <t>Web Service</t>
-  </si>
-  <si>
     <t>Buscador</t>
+  </si>
+  <si>
+    <t>Buscador Simple WS</t>
+  </si>
+  <si>
+    <t>Buscador Avanzado WS</t>
   </si>
 </sst>
 </file>
@@ -548,9 +545,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -573,6 +567,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,7 +669,7 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>542085</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>95460</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1380,7 +1377,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1433,34 +1430,34 @@
       <c r="W1" s="11"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="20">
         <v>2</v>
       </c>
-      <c r="C2" s="22">
-        <f t="shared" ref="C2:C12" si="0">B2*1</f>
+      <c r="C2" s="21">
+        <f t="shared" ref="C2" si="0">B2*1</f>
         <v>2</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="21">
         <v>4</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="20">
         <v>2</v>
       </c>
-      <c r="F2" s="21">
-        <v>1</v>
-      </c>
-      <c r="G2" s="21">
-        <f t="shared" ref="G2:G12" si="1">SUM(B2:F2)</f>
+      <c r="F2" s="20">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20">
+        <f t="shared" ref="G2" si="1">SUM(B2:F2)</f>
         <v>11</v>
       </c>
       <c r="H2" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I2" s="21">
-        <f t="shared" ref="I2:I12" si="2">G2*H2</f>
+      <c r="I2" s="20">
+        <f t="shared" ref="I2" si="2">G2*H2</f>
         <v>7.5460000000000003</v>
       </c>
       <c r="J2" s="2"/>
@@ -1469,34 +1466,34 @@
       <c r="W2" s="5"/>
     </row>
     <row r="3" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="21">
-        <v>0</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="B3" s="20">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21">
         <f t="shared" ref="C3:C28" si="3">B3*1</f>
         <v>0</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <f t="shared" ref="D3:D28" si="4">B3*1</f>
         <v>0</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="20">
         <v>4</v>
       </c>
-      <c r="F3" s="21">
-        <v>0</v>
-      </c>
-      <c r="G3" s="21">
+      <c r="F3" s="20">
+        <v>0</v>
+      </c>
+      <c r="G3" s="20">
         <f t="shared" ref="G3:G28" si="5">SUM(B3:F3)</f>
         <v>4</v>
       </c>
       <c r="H3" s="3">
         <v>0.57099999999999995</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <f t="shared" ref="I3:I28" si="6">G3*H3</f>
         <v>2.2839999999999998</v>
       </c>
@@ -1504,39 +1501,39 @@
       <c r="K3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B4" s="21">
-        <v>0</v>
-      </c>
-      <c r="C4" s="22">
+      <c r="B4" s="20">
+        <v>0</v>
+      </c>
+      <c r="C4" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E4" s="21">
-        <v>1</v>
-      </c>
-      <c r="F4" s="21">
-        <v>0</v>
-      </c>
-      <c r="G4" s="21">
+      <c r="E4" s="20">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H4" s="3">
         <v>0.57099999999999995</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <f t="shared" si="6"/>
         <v>0.57099999999999995</v>
       </c>
@@ -1549,34 +1546,34 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>2</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="E5" s="21">
-        <v>1</v>
-      </c>
-      <c r="F5" s="21">
-        <v>1</v>
-      </c>
-      <c r="G5" s="21">
+      <c r="E5" s="20">
+        <v>1</v>
+      </c>
+      <c r="F5" s="20">
+        <v>1</v>
+      </c>
+      <c r="G5" s="20">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="H5" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="20">
         <f t="shared" si="6"/>
         <v>5.4880000000000004</v>
       </c>
@@ -1589,34 +1586,34 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>7</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="E6" s="21">
-        <v>1</v>
-      </c>
-      <c r="F6" s="21">
-        <v>1</v>
-      </c>
-      <c r="G6" s="21">
+      <c r="E6" s="20">
+        <v>1</v>
+      </c>
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="H6" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <f t="shared" si="6"/>
         <v>15.778</v>
       </c>
@@ -1629,34 +1626,34 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>5</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="21">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="E7" s="21">
-        <v>1</v>
-      </c>
-      <c r="F7" s="21">
-        <v>1</v>
-      </c>
-      <c r="G7" s="21">
+      <c r="E7" s="20">
+        <v>1</v>
+      </c>
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="20">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
       <c r="H7" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="20">
         <f t="shared" si="6"/>
         <v>11.662000000000001</v>
       </c>
@@ -1669,34 +1666,34 @@
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="21">
-        <v>1</v>
-      </c>
-      <c r="C8" s="22">
+      <c r="B8" s="20">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="21">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>2</v>
       </c>
-      <c r="F8" s="21">
-        <v>1</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="20">
+        <v>1</v>
+      </c>
+      <c r="G8" s="20">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H8" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="20">
         <f t="shared" si="6"/>
         <v>4.1160000000000005</v>
       </c>
@@ -1709,34 +1706,34 @@
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="21">
-        <v>1</v>
-      </c>
-      <c r="C9" s="22">
+      <c r="B9" s="20">
+        <v>1</v>
+      </c>
+      <c r="C9" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="21">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>2</v>
       </c>
-      <c r="F9" s="21">
-        <v>1</v>
-      </c>
-      <c r="G9" s="21">
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H9" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <f t="shared" si="6"/>
         <v>4.1160000000000005</v>
       </c>
@@ -1749,589 +1746,595 @@
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="21">
-        <v>1</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="B10" s="20">
+        <v>1</v>
+      </c>
+      <c r="C10" s="21">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D10" s="21">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>2</v>
       </c>
-      <c r="F10" s="21">
-        <v>1</v>
-      </c>
-      <c r="G10" s="21">
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="H10" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <f t="shared" si="6"/>
         <v>4.1160000000000005</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="L10" s="28">
+      <c r="K10" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="L10" s="27">
         <v>0.96</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="20">
         <v>2</v>
       </c>
-      <c r="C11" s="22">
+      <c r="C11" s="21">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D11" s="21">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="20">
         <v>2</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="20">
         <v>2</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="20">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="H11" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <f t="shared" si="6"/>
         <v>6.86</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>7</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="21">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="21">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>2</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="20">
         <v>2</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="20">
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="H12" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <f t="shared" si="6"/>
         <v>17.150000000000002</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="21">
+      <c r="B13" s="20">
         <v>5</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="21">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="21">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <v>2</v>
       </c>
-      <c r="F13" s="21">
+      <c r="F13" s="20">
         <v>2</v>
       </c>
-      <c r="G13" s="21">
+      <c r="G13" s="20">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="H13" s="3">
         <v>0.68600000000000005</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <f t="shared" si="6"/>
         <v>13.034000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="21">
-        <v>0</v>
-      </c>
-      <c r="C14" s="22">
+      <c r="B14" s="20">
+        <v>0</v>
+      </c>
+      <c r="C14" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E14" s="21">
-        <v>1</v>
-      </c>
-      <c r="F14" s="21">
-        <v>0</v>
-      </c>
-      <c r="G14" s="21">
+      <c r="E14" s="20">
+        <v>1</v>
+      </c>
+      <c r="F14" s="20">
+        <v>0</v>
+      </c>
+      <c r="G14" s="20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H14" s="3">
         <v>0.57099999999999995</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="20">
         <f t="shared" si="6"/>
         <v>0.57099999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="21">
-        <v>0</v>
-      </c>
-      <c r="C15" s="22">
+      <c r="B15" s="20">
+        <v>0</v>
+      </c>
+      <c r="C15" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E15" s="21">
-        <v>1</v>
-      </c>
-      <c r="F15" s="21">
-        <v>0</v>
-      </c>
-      <c r="G15" s="21">
+      <c r="E15" s="20">
+        <v>1</v>
+      </c>
+      <c r="F15" s="20">
+        <v>0</v>
+      </c>
+      <c r="G15" s="20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H15" s="3">
         <v>0.57099999999999995</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <f t="shared" si="6"/>
         <v>0.57099999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="21">
-        <v>0</v>
-      </c>
-      <c r="C16" s="22">
+      <c r="B16" s="20">
+        <v>0</v>
+      </c>
+      <c r="C16" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="21">
-        <v>1</v>
-      </c>
-      <c r="F16" s="21">
-        <v>0</v>
-      </c>
-      <c r="G16" s="21">
+      <c r="E16" s="20">
+        <v>1</v>
+      </c>
+      <c r="F16" s="20">
+        <v>0</v>
+      </c>
+      <c r="G16" s="20">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="H16" s="3">
         <v>0.57099999999999995</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="20">
         <f t="shared" si="6"/>
         <v>0.57099999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22">
+      <c r="A17" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="21">
+        <v>2</v>
+      </c>
+      <c r="D17" s="21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="20">
+        <v>2</v>
+      </c>
+      <c r="F17" s="20">
+        <v>2</v>
+      </c>
+      <c r="G17" s="20">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.333</v>
+      </c>
+      <c r="I17" s="20">
+        <f t="shared" si="6"/>
+        <v>10.664</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="20">
+        <v>6</v>
+      </c>
+      <c r="C18" s="21">
+        <v>12</v>
+      </c>
+      <c r="D18" s="21">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="E18" s="20">
+        <v>2</v>
+      </c>
+      <c r="F18" s="20">
+        <v>1</v>
+      </c>
+      <c r="G18" s="20">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1.333</v>
+      </c>
+      <c r="I18" s="20">
+        <f t="shared" si="6"/>
+        <v>35.991</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D19" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21">
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H17" s="28">
-        <v>0.96</v>
-      </c>
-      <c r="I17" s="21">
+      <c r="H19" s="3"/>
+      <c r="I19" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22">
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D20" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21">
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H18" s="28">
-        <v>0.96</v>
-      </c>
-      <c r="I18" s="21">
+      <c r="H20" s="20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22">
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D21" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21">
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H19" s="3">
-        <v>1.333</v>
-      </c>
-      <c r="I19" s="21">
+      <c r="H21" s="20">
+        <v>0</v>
+      </c>
+      <c r="I21" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22">
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D22" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H20" s="21">
-        <v>0</v>
-      </c>
-      <c r="I20" s="21">
+      <c r="H22" s="20">
+        <v>0</v>
+      </c>
+      <c r="I22" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D23" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21">
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H21" s="21">
-        <v>0</v>
-      </c>
-      <c r="I21" s="21">
+      <c r="H23" s="20">
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D24" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21">
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H22" s="21">
-        <v>0</v>
-      </c>
-      <c r="I22" s="21">
+      <c r="H24" s="20">
+        <v>0</v>
+      </c>
+      <c r="I24" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D25" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H23" s="21">
-        <v>0</v>
-      </c>
-      <c r="I23" s="21">
+      <c r="H25" s="20">
+        <v>0</v>
+      </c>
+      <c r="I25" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D26" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H24" s="21">
-        <v>0</v>
-      </c>
-      <c r="I24" s="21">
+      <c r="H26" s="20">
+        <v>0</v>
+      </c>
+      <c r="I26" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D27" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H25" s="21">
-        <v>0</v>
-      </c>
-      <c r="I25" s="21">
+      <c r="H27" s="20">
+        <v>0</v>
+      </c>
+      <c r="I27" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D28" s="21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21">
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H26" s="21">
-        <v>0</v>
-      </c>
-      <c r="I26" s="21">
+      <c r="H28" s="20">
+        <v>0</v>
+      </c>
+      <c r="I28" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="21">
-        <v>0</v>
-      </c>
-      <c r="I27" s="21">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="22">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="21">
-        <v>0</v>
-      </c>
-      <c r="I28" s="21">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
       <c r="H30" s="12" t="s">
         <v>29</v>
       </c>
       <c r="I30" s="13">
         <f>SUM(I2:I28)</f>
-        <v>94.433999999999997</v>
+        <v>141.089</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C31" s="11"/>
       <c r="D31" s="11"/>
-      <c r="E31" s="26"/>
+      <c r="E31" s="25"/>
       <c r="H31" s="14" t="s">
         <v>30</v>
       </c>
       <c r="I31" s="15">
         <f>I30/8</f>
-        <v>11.80425</v>
+        <v>17.636125</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B32" s="16"/>
-      <c r="E32" s="26"/>
+      <c r="E32" s="25"/>
       <c r="H32" s="14" t="s">
         <v>33</v>
       </c>
       <c r="I32" s="15">
         <f>I30/'Calculo Costo Hora'!E2</f>
-        <v>2.3608500000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+        <v>3.5272250000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B33" s="16"/>
       <c r="E33" s="2"/>
       <c r="H33" s="14" t="s">
@@ -2339,7 +2342,7 @@
       </c>
       <c r="I33" s="15">
         <f>I32*'Calculo Costo Hora'!F12</f>
-        <v>1912288.5000000005</v>
+        <v>2857052.2500000005</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
@@ -2371,9 +2374,9 @@
     <mergeCell ref="B30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Detalles Empresa y fix estimación
</commit_message>
<xml_diff>
--- a/docPDS/Estimacion_Proyecto.xlsx
+++ b/docPDS/Estimacion_Proyecto.xlsx
@@ -32,7 +32,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="I32" authorId="0" shapeId="0">
+    <comment ref="I29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
   <si>
     <t>Número</t>
   </si>
@@ -277,18 +277,12 @@
     <t>Agregar Empresa</t>
   </si>
   <si>
-    <t>Eliminar Usuario</t>
-  </si>
-  <si>
     <t>Eliminar Persona</t>
   </si>
   <si>
     <t>Eliminar Empresa</t>
   </si>
   <si>
-    <t>Editar Usuario</t>
-  </si>
-  <si>
     <t>Editar Persona</t>
   </si>
   <si>
@@ -298,15 +292,9 @@
     <t>Listar Empresas</t>
   </si>
   <si>
-    <t>Listar Usuarios</t>
-  </si>
-  <si>
     <t>Listar Personas</t>
   </si>
   <si>
-    <t>Login Fallido</t>
-  </si>
-  <si>
     <t>Buscador</t>
   </si>
   <si>
@@ -314,6 +302,9 @@
   </si>
   <si>
     <t>Buscador Avanzado WS</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -486,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -553,9 +544,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -720,7 +708,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1373,11 +1361,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W39"/>
+  <dimension ref="A1:W36"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1473,11 +1461,11 @@
         <v>0</v>
       </c>
       <c r="C3" s="21">
-        <f t="shared" ref="C3:C28" si="3">B3*1</f>
+        <f t="shared" ref="C3:C25" si="3">B3*1</f>
         <v>0</v>
       </c>
       <c r="D3" s="21">
-        <f t="shared" ref="D3:D28" si="4">B3*1</f>
+        <f t="shared" ref="D3:D25" si="4">B3*1</f>
         <v>0</v>
       </c>
       <c r="E3" s="20">
@@ -1487,21 +1475,21 @@
         <v>0</v>
       </c>
       <c r="G3" s="20">
-        <f t="shared" ref="G3:G28" si="5">SUM(B3:F3)</f>
+        <f t="shared" ref="G3:G25" si="5">SUM(B3:F3)</f>
         <v>4</v>
       </c>
       <c r="H3" s="3">
-        <v>0.57099999999999995</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="I3" s="20">
-        <f t="shared" ref="I3:I28" si="6">G3*H3</f>
-        <v>2.2839999999999998</v>
+        <f t="shared" ref="I3:I25" si="6">G3*H3</f>
+        <v>2.7440000000000002</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="23" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1586,7 +1574,7 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="25" t="s">
         <v>60</v>
       </c>
       <c r="B6" s="20">
@@ -1750,55 +1738,55 @@
         <v>64</v>
       </c>
       <c r="B10" s="20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C10" s="21">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D10" s="21">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E10" s="20">
         <v>2</v>
       </c>
       <c r="F10" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="20">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H10" s="3">
         <v>0.68600000000000005</v>
       </c>
       <c r="I10" s="20">
         <f t="shared" si="6"/>
-        <v>4.1160000000000005</v>
+        <v>17.150000000000002</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="L10" s="27">
+      <c r="K10" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10" s="26">
         <v>0.96</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B11" s="20">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C11" s="21">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D11" s="21">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" s="20">
         <v>2</v>
@@ -1808,82 +1796,82 @@
       </c>
       <c r="G11" s="20">
         <f t="shared" si="5"/>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H11" s="3">
         <v>0.68600000000000005</v>
       </c>
       <c r="I11" s="20">
         <f t="shared" si="6"/>
-        <v>6.86</v>
+        <v>13.034000000000001</v>
       </c>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B12" s="20">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C12" s="21">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D12" s="21">
         <f t="shared" si="4"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E12" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="20">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="H12" s="3">
-        <v>0.68600000000000005</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="I12" s="20">
         <f t="shared" si="6"/>
-        <v>17.150000000000002</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="20">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C13" s="21">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D13" s="21">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" s="20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="20">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="H13" s="3">
-        <v>0.68600000000000005</v>
+        <v>0.57099999999999995</v>
       </c>
       <c r="I13" s="20">
         <f t="shared" si="6"/>
-        <v>13.034000000000001</v>
+        <v>0.57099999999999995</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
@@ -1891,74 +1879,68 @@
         <v>69</v>
       </c>
       <c r="B14" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="20">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H14" s="3">
-        <v>0.57099999999999995</v>
+        <v>1.333</v>
       </c>
       <c r="I14" s="20">
         <f t="shared" si="6"/>
-        <v>0.57099999999999995</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+        <v>10.664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C15" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D15" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E15" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="20">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="H15" s="3">
-        <v>0.57099999999999995</v>
+        <v>1.333</v>
       </c>
       <c r="I15" s="20">
         <f t="shared" si="6"/>
-        <v>0.57099999999999995</v>
+        <v>35.991</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="20">
-        <v>0</v>
-      </c>
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
       <c r="C16" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -1967,86 +1949,66 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="20">
-        <v>1</v>
-      </c>
-      <c r="F16" s="20">
-        <v>0</v>
-      </c>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="20">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.57099999999999995</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H16" s="3"/>
       <c r="I16" s="20">
         <f t="shared" si="6"/>
-        <v>0.57099999999999995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="20">
-        <v>1</v>
-      </c>
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="21">
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D17" s="21">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="E17" s="20">
-        <v>2</v>
-      </c>
-      <c r="F17" s="20">
-        <v>2</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="20">
         <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="H17" s="3">
-        <v>1.333</v>
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0</v>
       </c>
       <c r="I17" s="20">
         <f t="shared" si="6"/>
-        <v>10.664</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" s="20">
-        <v>6</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="21">
-        <v>12</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D18" s="21">
         <f t="shared" si="4"/>
-        <v>6</v>
-      </c>
-      <c r="E18" s="20">
-        <v>2</v>
-      </c>
-      <c r="F18" s="20">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="20">
         <f t="shared" si="5"/>
-        <v>27</v>
-      </c>
-      <c r="H18" s="3">
-        <v>1.333</v>
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
+        <v>0</v>
       </c>
       <c r="I18" s="20">
         <f t="shared" si="6"/>
-        <v>35.991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2066,7 +2028,9 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H19" s="3"/>
+      <c r="H19" s="20">
+        <v>0</v>
+      </c>
       <c r="I19" s="20">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2222,156 +2186,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D26" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="20">
-        <v>0</v>
-      </c>
-      <c r="I26" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D27" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H27" s="20">
-        <v>0</v>
-      </c>
-      <c r="I27" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="H27" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="13">
+        <f>SUM(I2:I25)</f>
+        <v>130.00200000000001</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="D28" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="H28" s="20">
-        <v>0</v>
-      </c>
-      <c r="I28" s="20">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="H30" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="13">
-        <f>SUM(I2:I28)</f>
-        <v>141.089</v>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="24"/>
+      <c r="H28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="15">
+        <f>I27/8</f>
+        <v>16.250250000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B29" s="16"/>
+      <c r="E29" s="24"/>
+      <c r="H29" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="15">
+        <f>I27/'Calculo Costo Hora'!E2</f>
+        <v>3.2500500000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B30" s="16"/>
+      <c r="E30" s="2"/>
+      <c r="H30" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="15">
+        <f>I29*'Calculo Costo Hora'!F12</f>
+        <v>2632540.5000000005</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="25"/>
-      <c r="H31" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="15">
-        <f>I30/8</f>
-        <v>17.636125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B31" s="16"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B32" s="16"/>
-      <c r="E32" s="25"/>
-      <c r="H32" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="15">
-        <f>I30/'Calculo Costo Hora'!E2</f>
-        <v>3.5272250000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="16"/>
       <c r="E33" s="2"/>
-      <c r="H33" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I33" s="15">
-        <f>I32*'Calculo Costo Hora'!F12</f>
-        <v>2857052.2500000005</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B34" s="16"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B35" s="16"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="16"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="16"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="16"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>